<commit_message>
dataclean add: knn_fillna, dataclean, output and data for test.
</commit_message>
<xml_diff>
--- a/codebook_year.xlsx
+++ b/codebook_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liang-yi/Documents/台大政研/資料分析與研究/masterthesis/MasterThesis_program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A92B593-CF9E-9A41-8CE0-C40D9420C0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4E13CD-0B7D-3B44-9BBA-94DCE33368B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{C5DF3351-D2BF-3647-A9EE-B04CE626E88E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20220" activeTab="1" xr2:uid="{C5DF3351-D2BF-3647-A9EE-B04CE626E88E}"/>
   </bookViews>
   <sheets>
     <sheet name="VAR" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>var</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +109,110 @@
   </si>
   <si>
     <t>notations</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,1,2,3,4,5,6,7,8,9,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N2A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N1B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>民主支持編成binary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,3,2,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>民主滿意反向編碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,90,95,96,98,99</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,1,1,2,0,0,0,0,0,0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泛藍1泛綠2中立無反應及其他0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>政治信任反向編碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>政治參與反向編碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女=0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251EA42E-0CF4-CF49-91E8-71B6A95F9DF0}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -496,65 +600,137 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -565,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B36EA1-0C59-E643-B4E0-7810F44A892F}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -587,6 +763,90 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>